<commit_message>
Update: September data files, GLS/Sameday/Netopia reports, and script improvements
- Add September GLS daily reports (22 files)
- Add September Sameday delivery reports (11 files)
- Add September Netopia batch files (4 files)
- Update eMag export files for August and September
- Update grupare facturi.py with latest changes
- Add debug scripts for OP matching
- Update config.txt

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/8_August/opuri_export.xlsx
+++ b/8_August/opuri_export.xlsx
@@ -3983,7 +3983,7 @@
     <row r="272">
       <c r="C272" t="inlineStr">
         <is>
-          <t>eMag Perioada 2025-07-16 - 2025-07-31 (nortia_dp_12823661_02_08_2025 (4).xlsx + nortia_dp_12823666_02_08_2025 (8).xlsx)</t>
+          <t>eMag Perioada 2025-07-16 - 2025-07-31 (nortia_dp_12823666_02_08_2025 (8).xlsx + nortia_dp_12823661_02_08_2025 (4).xlsx)</t>
         </is>
       </c>
       <c r="D272" s="2" t="inlineStr">
@@ -5451,7 +5451,7 @@
     <row r="343">
       <c r="C343" t="inlineStr">
         <is>
-          <t>eMag Perioada 2025-08-01 - 2025-08-15 (nortia_dp_12937396_17_08_2025 (1).xlsx + nortia_dp_12937390_17_08_2025 (1).xlsx)</t>
+          <t>eMag Perioada 2025-08-01 - 2025-08-15 (nortia_dp_12937390_17_08_2025 (1).xlsx + nortia_dp_12937396_17_08_2025 (1).xlsx)</t>
         </is>
       </c>
       <c r="D343" s="2" t="inlineStr">
@@ -6388,7 +6388,7 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>eMag Perioada 2025-08-16 - 2025-08-31 (nortia_dp_13052275_02_09_2025 (1).xlsx + nortia_dp_13052276_02_09_2025 (1).xlsx)</t>
+          <t>eMag Perioada 2025-08-16 - 2025-08-31 (nortia_dp_13052276_02_09_2025 (1).xlsx + nortia_dp_13052275_02_09_2025 (1).xlsx)</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">

</xml_diff>